<commit_message>
Suppression extension ToDispense d39cde71e2cf597d83e1549b12701eb13dce4047
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
+++ b/VoitureBalaisDecisions/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="112">
   <si>
     <t>Property</t>
   </si>
@@ -72,7 +72,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-14T13:55:20+00:00</t>
+    <t>2025-08-14T14:15:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -231,7 +231,10 @@
     <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Fourniture</t>
   </si>
   <si>
-    <t>MedicationRequest.medication[x].extension.valueBoolean</t>
+    <t>MedicationRequest.dispenseRequest.initialFill.quantity</t>
+  </si>
+  <si>
+    <t>not-related-to</t>
   </si>
   <si>
     <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Id_prescripteur</t>
@@ -271,9 +274,6 @@
   </si>
   <si>
     <t>MedicationRequest.dosageInstruction.timing.repeat.boundsPeriod.start</t>
-  </si>
-  <si>
-    <t>not-related-to</t>
   </si>
   <si>
     <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Dh_début</t>
@@ -1701,7 +1701,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1817,29 +1817,55 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
         <v>69</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1886,53 +1912,53 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1981,33 +2007,33 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -2063,24 +2089,24 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2094,7 +2120,7 @@
         <v>33</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -2117,7 +2143,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>